<commit_message>
add UT for use wid in Failure and Warning
</commit_message>
<xml_diff>
--- a/src/test/resources/data/in/jouerAuJeuDesLogos.xlsx
+++ b/src/test/resources/data/in/jouerAuJeuDesLogos.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="22">
   <si>
     <t>Résultat</t>
   </si>
@@ -77,6 +77,12 @@
   </si>
   <si>
     <t>score</t>
+  </si>
+  <si>
+    <t>Steven</t>
+  </si>
+  <si>
+    <t>heineken</t>
   </si>
 </sst>
 </file>
@@ -111,7 +117,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -130,6 +136,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -143,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -154,11 +166,75 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF6600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF6600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF6600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF6600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF6600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF6600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF6600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF6600"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF6600"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -484,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,16 +821,40 @@
       <c r="C24" s="8"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
+      <c r="A25" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
+      <c r="A26" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
+      <c r="A27" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="10"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
+      <c r="A28" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
@@ -823,19 +923,34 @@
       <c r="A50" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D9">
-    <cfRule type="expression" dxfId="2" priority="4">
+  <conditionalFormatting sqref="D9 D19">
+    <cfRule type="expression" dxfId="11" priority="10">
       <formula>COUNTIFS($A:$A,$A6,$D:$D, "Échec :*") &gt; 0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D19">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>COUNTIFS($A:$A,$A16,$D:$D, "Échec :*") &gt; 0</formula>
+  <conditionalFormatting sqref="D2:D5 D7:D8 D10:D18 D20:D24 A2:C24">
+    <cfRule type="expression" dxfId="9" priority="6">
+      <formula>COUNTIFS($A:$A,$A2,$D:$D, "Échec :*") &gt; 0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D5 D7:D8 D10:D18 D20:D24 A2:C24">
-    <cfRule type="expression" dxfId="0" priority="5">
-      <formula>COUNTIFS($A:$A,$A2,$D:$D, "Échec :*") &gt; 0</formula>
+  <conditionalFormatting sqref="B27">
+    <cfRule type="expression" dxfId="7" priority="4">
+      <formula>COUNTIFS($A:$A,$A26,$D:$D, "Échec :*") &gt; 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25:B25 B26 A26:A28">
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>COUNTIFS($A:$A,$A25,$D:$D, "Échec :*") &gt; 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B28">
+    <cfRule type="expression" dxfId="3" priority="2">
+      <formula>COUNTIFS($A:$A,$A28,$D:$D, "Échec :*") &gt; 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>COUNTIFS($A:$A,$A26,$D:$D, "Échec :*") &gt; 0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>